<commit_message>
refs #466 MS in Kriterienliste eingetragen
</commit_message>
<xml_diff>
--- a/doc/vorgaben/Kriterien SA SA-ElmerHeidtTreichler-ZuehlkePortfolioSurfaceV1.xlsx
+++ b/doc/vorgaben/Kriterien SA SA-ElmerHeidtTreichler-ZuehlkePortfolioSurfaceV1.xlsx
@@ -641,7 +641,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -846,6 +846,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -998,7 +1004,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1109,9 +1115,6 @@
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1210,6 +1213,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3727,7 +3742,7 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3736,21 +3751,21 @@
     <col min="2" max="2" width="120.85546875" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="56.28515625" style="62" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="74" customWidth="1"/>
+    <col min="5" max="5" width="56.28515625" style="61" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="73" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="74"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="73"/>
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A2" s="3"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="74"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="73"/>
     </row>
     <row r="3" spans="1:6" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A3" s="24" t="s">
@@ -3763,11 +3778,11 @@
       <c r="D3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="64">
+      <c r="E3" s="63">
         <f>SUMPRODUCT(Table2[G],Table2[N])/SUM(Table2[G])</f>
         <v>0</v>
       </c>
-      <c r="F3" s="74"/>
+      <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A4" s="29" t="s">
@@ -3801,7 +3816,7 @@
       </c>
       <c r="D5" s="41"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="75"/>
+      <c r="F5" s="74"/>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A6" s="31">
@@ -3815,7 +3830,7 @@
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="42"/>
-      <c r="F6" s="75"/>
+      <c r="F6" s="74"/>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A7" s="31">
@@ -3828,10 +3843,10 @@
         <v>5</v>
       </c>
       <c r="D7" s="41"/>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="75"/>
+      <c r="F7" s="74"/>
     </row>
     <row r="8" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A8" s="5">
@@ -3845,7 +3860,7 @@
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="43"/>
-      <c r="F8" s="76">
+      <c r="F8" s="75">
         <v>40812</v>
       </c>
     </row>
@@ -3861,7 +3876,9 @@
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="43"/>
-      <c r="F9" s="75"/>
+      <c r="F9" s="75">
+        <v>40819</v>
+      </c>
     </row>
     <row r="10" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A10" s="9">
@@ -3875,7 +3892,9 @@
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="43"/>
-      <c r="F10" s="75"/>
+      <c r="F10" s="75">
+        <v>40819</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A11" s="9">
@@ -3889,7 +3908,9 @@
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="43"/>
-      <c r="F11" s="75"/>
+      <c r="F11" s="75">
+        <v>40819</v>
+      </c>
     </row>
     <row r="12" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A12" s="5">
@@ -3903,7 +3924,7 @@
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="43"/>
-      <c r="F12" s="75"/>
+      <c r="F12" s="74"/>
     </row>
     <row r="13" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A13" s="5">
@@ -3917,7 +3938,7 @@
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="43"/>
-      <c r="F13" s="75"/>
+      <c r="F13" s="74"/>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A14" s="5">
@@ -3933,7 +3954,7 @@
       <c r="E14" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="F14" s="75"/>
+      <c r="F14" s="74"/>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A15" s="9">
@@ -3947,7 +3968,7 @@
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="43"/>
-      <c r="F15" s="75"/>
+      <c r="F15" s="74"/>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A16" s="9">
@@ -3961,7 +3982,7 @@
       </c>
       <c r="D16" s="33"/>
       <c r="E16" s="43"/>
-      <c r="F16" s="75"/>
+      <c r="F16" s="74"/>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="5">
@@ -3975,7 +3996,7 @@
       </c>
       <c r="D17" s="33"/>
       <c r="E17" s="43"/>
-      <c r="F17" s="75"/>
+      <c r="F17" s="74"/>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A18" s="5">
@@ -3989,7 +4010,7 @@
       </c>
       <c r="D18" s="33"/>
       <c r="E18" s="43"/>
-      <c r="F18" s="75"/>
+      <c r="F18" s="74"/>
     </row>
     <row r="19" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A19" s="25">
@@ -4003,7 +4024,7 @@
       </c>
       <c r="D19" s="33"/>
       <c r="E19" s="42"/>
-      <c r="F19" s="75"/>
+      <c r="F19" s="74"/>
     </row>
     <row r="20" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A20" s="30">
@@ -4017,7 +4038,7 @@
       </c>
       <c r="D20" s="33"/>
       <c r="E20" s="43"/>
-      <c r="F20" s="75"/>
+      <c r="F20" s="74"/>
     </row>
     <row r="21" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A21" s="25">
@@ -4031,7 +4052,7 @@
       </c>
       <c r="D21" s="33"/>
       <c r="E21" s="43"/>
-      <c r="F21" s="75"/>
+      <c r="F21" s="74"/>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A22" s="25">
@@ -4047,7 +4068,7 @@
       <c r="E22" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="F22" s="75"/>
+      <c r="F22" s="74"/>
     </row>
     <row r="23" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A23" s="25">
@@ -4061,7 +4082,7 @@
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="43"/>
-      <c r="F23" s="75"/>
+      <c r="F23" s="74"/>
     </row>
     <row r="24" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A24" s="25">
@@ -4075,7 +4096,7 @@
       </c>
       <c r="D24" s="33"/>
       <c r="E24" s="43"/>
-      <c r="F24" s="75"/>
+      <c r="F24" s="74"/>
     </row>
     <row r="25" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A25" s="25">
@@ -4089,21 +4110,21 @@
       </c>
       <c r="D25" s="33"/>
       <c r="E25" s="43"/>
-      <c r="F25" s="75"/>
+      <c r="F25" s="74"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>22</v>
       </c>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="61" t="s">
         <v>157</v>
       </c>
       <c r="C26" s="40">
         <v>5</v>
       </c>
       <c r="D26" s="33"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="75"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="74"/>
     </row>
     <row r="27" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A27" s="25">
@@ -4117,7 +4138,7 @@
       </c>
       <c r="D27" s="33"/>
       <c r="E27" s="43"/>
-      <c r="F27" s="75"/>
+      <c r="F27" s="74"/>
     </row>
     <row r="28" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A28" s="25">
@@ -4133,7 +4154,7 @@
       <c r="E28" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="F28" s="75"/>
+      <c r="F28" s="74"/>
     </row>
     <row r="29" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A29" s="25">
@@ -4147,7 +4168,7 @@
       </c>
       <c r="D29" s="33"/>
       <c r="E29" s="43"/>
-      <c r="F29" s="75"/>
+      <c r="F29" s="74"/>
     </row>
     <row r="30" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A30" s="25">
@@ -4163,7 +4184,7 @@
       <c r="E30" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="F30" s="75"/>
+      <c r="F30" s="74"/>
     </row>
     <row r="31" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A31" s="25">
@@ -4177,7 +4198,7 @@
       </c>
       <c r="D31" s="33"/>
       <c r="E31" s="43"/>
-      <c r="F31" s="75"/>
+      <c r="F31" s="74"/>
     </row>
     <row r="32" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A32" s="21">
@@ -4191,28 +4212,29 @@
       </c>
       <c r="D32" s="41"/>
       <c r="E32" s="42"/>
-      <c r="F32" s="75"/>
+      <c r="F32" s="74"/>
     </row>
     <row r="33" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A33" s="59">
+      <c r="A33" s="58">
         <v>29</v>
       </c>
-      <c r="B33" s="60" t="s">
+      <c r="B33" s="59" t="s">
         <v>159</v>
       </c>
       <c r="C33" s="40">
         <v>5</v>
       </c>
       <c r="D33" s="44"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="75"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="74"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="47"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="82"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="85"/>
     </row>
     <row r="35" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
@@ -4224,7 +4246,7 @@
       <c r="D35" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="64">
+      <c r="E35" s="63">
         <f>SUMPRODUCT(Table6[G],Table6[N])/SUM(Table6[G])</f>
         <v>0</v>
       </c>
@@ -4258,10 +4280,10 @@
         <v>5</v>
       </c>
       <c r="D37" s="33"/>
-      <c r="E37" s="47" t="s">
+      <c r="E37" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="F37" s="74"/>
+      <c r="F37" s="73"/>
     </row>
     <row r="38" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A38" s="12">
@@ -4275,7 +4297,7 @@
       </c>
       <c r="D38" s="33"/>
       <c r="E38" s="42"/>
-      <c r="F38" s="74"/>
+      <c r="F38" s="73"/>
     </row>
     <row r="39" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A39" s="12">
@@ -4291,7 +4313,7 @@
       <c r="E39" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="F39" s="74"/>
+      <c r="F39" s="73"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
@@ -4398,12 +4420,12 @@
       <c r="E47" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="F47" s="74"/>
+      <c r="F47" s="73"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
-      <c r="E48" s="67"/>
+      <c r="E48" s="66"/>
     </row>
     <row r="49" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A49" s="23" t="s">
@@ -4416,7 +4438,7 @@
       <c r="D49" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="64">
+      <c r="E49" s="63">
         <f>SUMPRODUCT(Table12[G],Table12[N])/SUM(Table12[G])</f>
         <v>0</v>
       </c>
@@ -4449,7 +4471,7 @@
         <v>5</v>
       </c>
       <c r="D51" s="33"/>
-      <c r="E51" s="68"/>
+      <c r="E51" s="67"/>
     </row>
     <row r="52" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
@@ -4463,7 +4485,7 @@
       </c>
       <c r="D52" s="33"/>
       <c r="E52" s="38"/>
-      <c r="F52" s="74"/>
+      <c r="F52" s="73"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
@@ -4489,7 +4511,7 @@
         <v>5</v>
       </c>
       <c r="D54" s="33"/>
-      <c r="E54" s="53"/>
+      <c r="E54" s="52"/>
       <c r="F54" s="26"/>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4521,7 +4543,7 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
-      <c r="E57" s="67"/>
+      <c r="E57" s="66"/>
     </row>
     <row r="58" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A58" s="23" t="s">
@@ -4534,7 +4556,7 @@
       <c r="D58" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E58" s="64">
+      <c r="E58" s="63">
         <f>SUMPRODUCT(Table3[G],Table3[N])/SUM(Table3[G])</f>
         <v>0</v>
       </c>
@@ -4644,7 +4666,7 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
-      <c r="E66" s="67"/>
+      <c r="E66" s="66"/>
     </row>
     <row r="67" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A67" s="23" t="s">
@@ -4656,7 +4678,7 @@
       <c r="D67" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E67" s="64">
+      <c r="E67" s="63">
         <f>SUMPRODUCT(Table11[G],Table11[N])/SUM(Table11[G])</f>
         <v>0</v>
       </c>
@@ -4749,12 +4771,12 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
-      <c r="E74" s="67"/>
+      <c r="E74" s="66"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
-      <c r="E75" s="67"/>
+      <c r="E75" s="66"/>
     </row>
     <row r="76" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A76" s="23" t="s">
@@ -4766,7 +4788,7 @@
       <c r="D76" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E76" s="64">
+      <c r="E76" s="63">
         <f>SUMPRODUCT(Table71518[G],Table71518[N])/SUM(Table71518[G])</f>
         <v>0</v>
       </c>
@@ -4858,7 +4880,7 @@
       <c r="B84"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
-      <c r="E84" s="69"/>
+      <c r="E84" s="68"/>
       <c r="F84" s="26"/>
     </row>
     <row r="85" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -4872,7 +4894,7 @@
       <c r="D85" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E85" s="64">
+      <c r="E85" s="63">
         <f>SUMPRODUCT(Table715[G],Table715[N])/SUM(Table715[G])</f>
         <v>0</v>
       </c>
@@ -4976,7 +4998,7 @@
       <c r="B93"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
-      <c r="E93" s="69"/>
+      <c r="E93" s="68"/>
       <c r="F93" s="26"/>
     </row>
     <row r="94" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -4990,7 +5012,7 @@
       <c r="D94" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E94" s="64">
+      <c r="E94" s="63">
         <f>SUMPRODUCT(Table7[G],Table7[N])/SUM(Table7[G])</f>
         <v>0</v>
       </c>
@@ -5119,10 +5141,10 @@
       <c r="E103" s="38"/>
     </row>
     <row r="104" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B104" s="57"/>
+      <c r="B104" s="56"/>
       <c r="C104" s="34"/>
-      <c r="D104" s="58"/>
-      <c r="E104" s="70"/>
+      <c r="D104" s="57"/>
+      <c r="E104" s="69"/>
       <c r="F104" s="26"/>
     </row>
     <row r="105" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5136,7 +5158,7 @@
       <c r="D105" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="64">
+      <c r="E105" s="63">
         <f>SUMPRODUCT(Table8[G],Table8[N])/SUM(Table8[G])</f>
         <v>0</v>
       </c>
@@ -5182,7 +5204,7 @@
         <v>5</v>
       </c>
       <c r="D108" s="33"/>
-      <c r="E108" s="68"/>
+      <c r="E108" s="67"/>
     </row>
     <row r="109" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
@@ -5211,10 +5233,10 @@
       <c r="E110" s="38"/>
     </row>
     <row r="111" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B111" s="57"/>
+      <c r="B111" s="56"/>
       <c r="C111" s="34"/>
-      <c r="D111" s="58"/>
-      <c r="E111" s="70"/>
+      <c r="D111" s="57"/>
+      <c r="E111" s="69"/>
       <c r="F111" s="26"/>
     </row>
     <row r="112" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5228,7 +5250,7 @@
       <c r="D112" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E112" s="64">
+      <c r="E112" s="63">
         <f>SUMPRODUCT(Table9[G],Table9[N])/SUM(Table9[G])</f>
         <v>0</v>
       </c>
@@ -5358,7 +5380,7 @@
       <c r="B122"/>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
-      <c r="E122" s="69"/>
+      <c r="E122" s="68"/>
       <c r="F122" s="26"/>
     </row>
     <row r="123" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5372,7 +5394,7 @@
       <c r="D123" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E123" s="64">
+      <c r="E123" s="63">
         <f>SUMPRODUCT(Table1021[G],Table1021[N])/SUM(Table1021[G])</f>
         <v>0</v>
       </c>
@@ -5437,7 +5459,7 @@
       <c r="A128" s="9">
         <v>4</v>
       </c>
-      <c r="B128" s="57" t="s">
+      <c r="B128" s="56" t="s">
         <v>134</v>
       </c>
       <c r="C128" s="34">
@@ -5493,7 +5515,7 @@
       <c r="A132" s="5">
         <v>8</v>
       </c>
-      <c r="B132" s="57" t="s">
+      <c r="B132" s="56" t="s">
         <v>135</v>
       </c>
       <c r="C132" s="34">
@@ -5534,7 +5556,7 @@
       <c r="B135"/>
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
-      <c r="E135" s="69"/>
+      <c r="E135" s="68"/>
       <c r="F135" s="26"/>
     </row>
     <row r="136" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5548,7 +5570,7 @@
       <c r="D136" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E136" s="64">
+      <c r="E136" s="63">
         <f>SUMPRODUCT(Table1020[G],Table1020[N])/SUM(Table1020[G])</f>
         <v>0</v>
       </c>
@@ -5623,17 +5645,17 @@
       <c r="E141" s="38"/>
     </row>
     <row r="142" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A142" s="77">
-        <v>5</v>
-      </c>
-      <c r="B142" s="78" t="s">
+      <c r="A142" s="76">
+        <v>5</v>
+      </c>
+      <c r="B142" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="C142" s="79">
+      <c r="C142" s="78">
         <v>0</v>
       </c>
-      <c r="D142" s="80"/>
-      <c r="E142" s="81" t="s">
+      <c r="D142" s="79"/>
+      <c r="E142" s="80" t="s">
         <v>177</v>
       </c>
     </row>
@@ -5679,13 +5701,13 @@
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
-      <c r="E146" s="67"/>
+      <c r="E146" s="66"/>
     </row>
     <row r="147" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
-      <c r="E147" s="69"/>
+      <c r="E147" s="68"/>
       <c r="F147" s="26"/>
     </row>
     <row r="148" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5699,7 +5721,7 @@
       <c r="D148" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E148" s="64">
+      <c r="E148" s="63">
         <f>SUMPRODUCT(Table10[G],Table10[N])/SUM(Table10[G])</f>
         <v>0</v>
       </c>
@@ -5799,7 +5821,7 @@
         <v>5</v>
       </c>
       <c r="D155" s="33"/>
-      <c r="E155" s="53"/>
+      <c r="E155" s="52"/>
     </row>
     <row r="156" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="9">
@@ -5842,7 +5864,7 @@
         <v>5</v>
       </c>
       <c r="D158" s="33"/>
-      <c r="E158" s="53"/>
+      <c r="E158" s="52"/>
     </row>
     <row r="159" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="9">
@@ -5871,7 +5893,7 @@
       <c r="E160" s="38"/>
     </row>
     <row r="161" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="61">
+      <c r="A161" s="60">
         <v>12</v>
       </c>
       <c r="B161" s="2" t="s">
@@ -5912,7 +5934,7 @@
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
-      <c r="E164" s="67"/>
+      <c r="E164" s="66"/>
     </row>
     <row r="165" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A165" s="23" t="s">
@@ -5925,7 +5947,7 @@
       <c r="D165" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E165" s="64">
+      <c r="E165" s="63">
         <f>SUMPRODUCT(Table15[G],Table15[N])/SUM(Table15[G])</f>
         <v>0</v>
       </c>
@@ -5992,7 +6014,7 @@
       <c r="A170" s="9">
         <v>4</v>
       </c>
-      <c r="B170" s="57" t="s">
+      <c r="B170" s="56" t="s">
         <v>129</v>
       </c>
       <c r="C170" s="34">
@@ -6004,14 +6026,14 @@
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
-      <c r="E171" s="67"/>
-    </row>
-    <row r="173" spans="1:6" s="56" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A173" s="55" t="s">
+      <c r="E171" s="66"/>
+    </row>
+    <row r="173" spans="1:6" s="55" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A173" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="E173" s="71"/>
-      <c r="F173" s="82" t="s">
+      <c r="E173" s="70"/>
+      <c r="F173" s="81" t="s">
         <v>182</v>
       </c>
     </row>
@@ -6026,311 +6048,311 @@
       <c r="D174" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E174" s="64">
+      <c r="E174" s="63">
         <f>SUMPRODUCT(Table2[G],Table2[N])/SUM(Table2[G])</f>
         <v>0</v>
       </c>
-      <c r="F174" s="82">
+      <c r="F174" s="81">
         <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F175" s="82"/>
+      <c r="F175" s="81"/>
     </row>
     <row r="176" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A176" s="50" t="s">
+      <c r="A176" s="49" t="s">
         <v>87</v>
       </c>
       <c r="B176" s="10" t="s">
         <v>63</v>
       </c>
       <c r="C176" s="10"/>
-      <c r="D176" s="51" t="s">
+      <c r="D176" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E176" s="72">
+      <c r="E176" s="71">
         <f>SUMPRODUCT(Table6[G],Table6[N])/SUM(Table6[G])</f>
         <v>0</v>
       </c>
-      <c r="F176" s="82">
+      <c r="F176" s="81">
         <v>3</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A177" s="50" t="s">
+      <c r="A177" s="49" t="s">
         <v>88</v>
       </c>
       <c r="B177" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C177" s="10"/>
-      <c r="D177" s="51" t="s">
+      <c r="D177" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E177" s="72">
+      <c r="E177" s="71">
         <f>SUMPRODUCT(Table12[G],Table12[N])/SUM(Table12[G])</f>
         <v>0</v>
       </c>
-      <c r="F177" s="82">
+      <c r="F177" s="81">
         <v>3</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A178" s="50" t="s">
+      <c r="A178" s="49" t="s">
         <v>89</v>
       </c>
       <c r="B178" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C178" s="10"/>
-      <c r="D178" s="51" t="s">
+      <c r="D178" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E178" s="72">
+      <c r="E178" s="71">
         <f>SUMPRODUCT(Table3[G],Table3[N])/SUM(Table3[G])</f>
         <v>0</v>
       </c>
-      <c r="F178" s="82">
+      <c r="F178" s="81">
         <v>3</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A179" s="48">
+      <c r="A179" s="47">
         <v>2</v>
       </c>
-      <c r="B179" s="49" t="s">
+      <c r="B179" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="E179" s="73">
+      <c r="E179" s="72">
         <f>SUMPRODUCT(F176:F178,E176:E178)/SUM(F176:F178)</f>
         <v>0</v>
       </c>
-      <c r="F179" s="82">
+      <c r="F179" s="81">
         <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F180" s="82"/>
+      <c r="F180" s="81"/>
     </row>
     <row r="181" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A181" s="50" t="s">
+      <c r="A181" s="49" t="s">
         <v>77</v>
       </c>
       <c r="B181" s="10" t="s">
         <v>74</v>
       </c>
       <c r="C181" s="10"/>
-      <c r="D181" s="51" t="s">
+      <c r="D181" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E181" s="72">
+      <c r="E181" s="71">
         <f>SUMPRODUCT(Table11[G],Table11[N])/SUM(Table11[G])</f>
         <v>0</v>
       </c>
-      <c r="F181" s="82">
+      <c r="F181" s="81">
         <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A182" s="50" t="s">
+      <c r="A182" s="49" t="s">
         <v>78</v>
       </c>
       <c r="B182" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C182" s="10"/>
-      <c r="D182" s="51" t="s">
+      <c r="D182" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E182" s="72">
+      <c r="E182" s="71">
         <f>SUMPRODUCT(Table71518[G],Table71518[N])/SUM(Table71518[G])</f>
         <v>0</v>
       </c>
-      <c r="F182" s="82">
+      <c r="F182" s="81">
         <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A183" s="50" t="s">
+      <c r="A183" s="49" t="s">
         <v>79</v>
       </c>
       <c r="B183" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C183" s="10"/>
-      <c r="D183" s="51" t="s">
+      <c r="D183" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E183" s="72">
+      <c r="E183" s="71">
         <f>SUMPRODUCT(Table715[G],Table715[N])/SUM(Table715[G])</f>
         <v>0</v>
       </c>
-      <c r="F183" s="82">
+      <c r="F183" s="81">
         <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A184" s="50" t="s">
+      <c r="A184" s="49" t="s">
         <v>80</v>
       </c>
       <c r="B184" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C184" s="10"/>
-      <c r="D184" s="51" t="s">
+      <c r="D184" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E184" s="72">
+      <c r="E184" s="71">
         <f>SUMPRODUCT(Table7[G],Table7[N])/SUM(Table7[G])</f>
         <v>0</v>
       </c>
-      <c r="F184" s="82">
+      <c r="F184" s="81">
         <v>6</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A185" s="50" t="s">
+      <c r="A185" s="49" t="s">
         <v>81</v>
       </c>
       <c r="B185" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C185" s="10"/>
-      <c r="D185" s="51" t="s">
+      <c r="D185" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E185" s="72">
+      <c r="E185" s="71">
         <f>SUMPRODUCT(Table8[G],Table8[N])/SUM(Table8[G])</f>
         <v>0</v>
       </c>
-      <c r="F185" s="82">
+      <c r="F185" s="81">
         <v>3</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A186" s="50" t="s">
+      <c r="A186" s="49" t="s">
         <v>99</v>
       </c>
       <c r="B186" s="10" t="s">
         <v>101</v>
       </c>
       <c r="C186" s="10"/>
-      <c r="D186" s="51" t="s">
+      <c r="D186" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E186" s="72">
+      <c r="E186" s="71">
         <f>SUMPRODUCT(Table9[G],Table9[N])/SUM(Table9[G])</f>
         <v>0</v>
       </c>
-      <c r="F186" s="82">
+      <c r="F186" s="81">
         <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A187" s="50" t="s">
+      <c r="A187" s="49" t="s">
         <v>82</v>
       </c>
       <c r="B187" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C187" s="10"/>
-      <c r="D187" s="51" t="s">
+      <c r="D187" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E187" s="72">
+      <c r="E187" s="71">
         <f>SUMPRODUCT(Table1021[G],Table1021[N])/SUM(Table1021[G])</f>
         <v>0</v>
       </c>
-      <c r="F187" s="82">
+      <c r="F187" s="81">
         <v>6</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A188" s="50" t="s">
+      <c r="A188" s="49" t="s">
         <v>83</v>
       </c>
       <c r="B188" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C188" s="10"/>
-      <c r="D188" s="51" t="s">
+      <c r="D188" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E188" s="72">
+      <c r="E188" s="71">
         <f>SUMPRODUCT(Table1020[G],Table1020[N])/SUM(Table1020[G])</f>
         <v>0</v>
       </c>
-      <c r="F188" s="82">
+      <c r="F188" s="81">
         <v>2</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A189" s="50" t="s">
+      <c r="A189" s="49" t="s">
         <v>84</v>
       </c>
       <c r="B189" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C189" s="10"/>
-      <c r="D189" s="51" t="s">
+      <c r="D189" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E189" s="72">
+      <c r="E189" s="71">
         <f>SUMPRODUCT(Table10[G],Table10[N])/SUM(Table10[G])</f>
         <v>0</v>
       </c>
-      <c r="F189" s="82">
+      <c r="F189" s="81">
         <v>2</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A190" s="50" t="s">
+      <c r="A190" s="49" t="s">
         <v>85</v>
       </c>
       <c r="B190" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C190" s="52"/>
-      <c r="D190" s="51" t="s">
+      <c r="C190" s="51"/>
+      <c r="D190" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E190" s="72">
+      <c r="E190" s="71">
         <v>0</v>
       </c>
-      <c r="F190" s="82">
+      <c r="F190" s="81">
         <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A191" s="48">
+      <c r="A191" s="47">
         <v>2</v>
       </c>
-      <c r="B191" s="49" t="s">
+      <c r="B191" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="E191" s="73">
+      <c r="E191" s="72">
         <f>SUMPRODUCT(F181:F190,E181:E190)/SUM(F181:F190)</f>
         <v>0</v>
       </c>
-      <c r="F191" s="82">
+      <c r="F191" s="81">
         <v>3</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F192" s="82"/>
+      <c r="F192" s="81"/>
     </row>
     <row r="193" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F193" s="82"/>
+      <c r="F193" s="81"/>
     </row>
     <row r="194" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
         <v>102</v>
       </c>
-      <c r="E194" s="62">
+      <c r="E194" s="61">
         <f>((E174*F174)+E179*F179+E191*F191)/(F174+F179+F191)</f>
         <v>0</v>
       </c>
-      <c r="F194" s="82"/>
+      <c r="F194" s="81"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">

</xml_diff>

<commit_message>
refs #457 Sprint Planung Sprint 7
</commit_message>
<xml_diff>
--- a/doc/vorgaben/Kriterien SA SA-ElmerHeidtTreichler-ZuehlkePortfolioSurfaceV1.xlsx
+++ b/doc/vorgaben/Kriterien SA SA-ElmerHeidtTreichler-ZuehlkePortfolioSurfaceV1.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="196">
   <si>
     <t>#</t>
   </si>
@@ -531,12 +531,6 @@
     <t>2 Dokumente (Bericht und Technischer Teil) mit gleicher Seitennummerierung sind ok</t>
   </si>
   <si>
-    <t>empfehlenswert (üben für Bachelorarbeit)</t>
-  </si>
-  <si>
-    <t>Management Summary</t>
-  </si>
-  <si>
     <t>Komplexität von Project Flip 2.0 ist hoch</t>
   </si>
   <si>
@@ -586,9 +580,6 @@
     <t>Inhaltsverzeichnis mit HTML nicht nötig, sofern gut beschriftete Ordner</t>
   </si>
   <si>
-    <t>Association for Computer Machinery, acm.org</t>
-  </si>
-  <si>
     <t>enthält Problemstellung und Demo. Demo auch auf Bildschrim möglich (falls Surface2 nicht vorhanden)</t>
   </si>
   <si>
@@ -632,6 +623,56 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Resultat Metrik-Auswertung</t>
+  </si>
+  <si>
+    <t>was wird alles an Software benötigt für Checkout</t>
+  </si>
+  <si>
+    <t>Schreiben was man mit Unit Tests testen will</t>
+  </si>
+  <si>
+    <t>Package Dependency Übersicht sehr wichtig. Dependency berechnen mit NDepend (ev Plugin Resharper).</t>
+  </si>
+  <si>
+    <t>Abnahme-Sitzung zu jedem Sprint inkl. Abnahmedokument (z.B. was verschoben+wieso).</t>
+  </si>
+  <si>
+    <t>Farbenblindheit (Check mit Farben)</t>
+  </si>
+  <si>
+    <t>Falls es mehrere Screen gibt braucht es ein Navigation Map</t>
+  </si>
+  <si>
+    <t>Dokument für Anforderungsspezifikation mit Liste der User Stories</t>
+  </si>
+  <si>
+    <t>Konkurrenz ist bestehende Lösung (Papier)</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Brochure Text = Management Summary</t>
+  </si>
+  <si>
+    <t>empfehlenswert (üben für Bachelorarbeit), kann auch nach Abgabe erstellt werden von allem anderen</t>
+  </si>
+  <si>
+    <t>Evt. mit Präsentation der Arbeit ink. Feedback</t>
+  </si>
+  <si>
+    <t>Verschiedene Zielgruppen bei Abstract, Management Summaries (jemand von aussen der sich detailiert informieren will mit Fokus auf Business Value), Technischer Report (für Leute mit technischem Hintergrund), Projektdokumente für Maitenance.
+Management Summary: Nicht mehr Text als in Abstract. Die Vision kann auf Management Summary verweisen.
+Extended Management Summary: In Dokument ist länger als Management Summary. Damit man gut versteht was gemacht wurde. Etwa 2-4 Seiten</t>
+  </si>
+  <si>
+    <t>Association for Computer Machinery, acm.org, Punkt wird verlangt. Paper raussuchen zu unserem Thema</t>
   </si>
 </sst>
 </file>
@@ -641,7 +682,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -852,6 +893,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF505050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -861,7 +909,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -875,6 +923,15 @@
       <top/>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1004,7 +1061,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1226,6 +1283,18 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="123">
@@ -1353,7 +1422,7 @@
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="113">
+  <dxfs count="115">
     <dxf>
       <font>
         <b val="0"/>
@@ -1520,6 +1589,24 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1827,6 +1914,24 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3253,197 +3358,199 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A59:E65" totalsRowShown="0" headerRowDxfId="112" tableBorderDxfId="111">
-  <autoFilter ref="A59:E65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A60:E66" totalsRowShown="0" headerRowDxfId="114" tableBorderDxfId="113">
+  <autoFilter ref="A60:E66"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="110"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="109"/>
-    <tableColumn id="5" name="G" dataDxfId="108"/>
-    <tableColumn id="3" name="N" dataDxfId="107"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="106"/>
+    <tableColumn id="1" name="#" dataDxfId="112"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="111"/>
+    <tableColumn id="5" name="G" dataDxfId="110"/>
+    <tableColumn id="3" name="N" dataDxfId="109"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:F34" totalsRowCount="1" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:F34" totalsRowCount="1" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42">
   <autoFilter ref="A4:F33"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="39" totalsRowDxfId="5"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="38" totalsRowDxfId="4"/>
-    <tableColumn id="6" name="G" dataDxfId="37" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="N" dataDxfId="36" totalsRowDxfId="2"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="35" totalsRowDxfId="1"/>
-    <tableColumn id="5" name="besprochen am" dataDxfId="34" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="41" totalsRowDxfId="5"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="40" totalsRowDxfId="4"/>
+    <tableColumn id="6" name="G" dataDxfId="39" totalsRowDxfId="3"/>
+    <tableColumn id="3" name="N" dataDxfId="38" totalsRowDxfId="2"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="37" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="besprochen am" dataDxfId="36" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table715" displayName="Table715" ref="A86:E92" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
-  <autoFilter ref="A86:E92"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="30"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="29"/>
-    <tableColumn id="5" name="G" dataDxfId="28"/>
-    <tableColumn id="3" name="N" dataDxfId="27"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table715" displayName="Table715" ref="A87:F93" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33">
+  <autoFilter ref="A87:F93"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="#" dataDxfId="32"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="31"/>
+    <tableColumn id="5" name="G" dataDxfId="30"/>
+    <tableColumn id="3" name="N" dataDxfId="29"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="28"/>
+    <tableColumn id="6" name="Column1" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table71518" displayName="Table71518" ref="A77:E82" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23">
-  <autoFilter ref="A77:E82"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="22"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="21"/>
-    <tableColumn id="5" name="G" dataDxfId="20"/>
-    <tableColumn id="3" name="N" dataDxfId="19"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table71518" displayName="Table71518" ref="A78:F83" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24">
+  <autoFilter ref="A78:F83"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="#" dataDxfId="23"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="22"/>
+    <tableColumn id="5" name="G" dataDxfId="21"/>
+    <tableColumn id="3" name="N" dataDxfId="20"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="19"/>
+    <tableColumn id="6" name="Column1" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1020" displayName="Table1020" ref="A137:E145" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A137:E145"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1020" displayName="Table1020" ref="A138:E146" totalsRowShown="0" headerRowDxfId="18">
+  <autoFilter ref="A138:E146"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="16"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="15"/>
-    <tableColumn id="5" name="G" dataDxfId="14"/>
-    <tableColumn id="3" name="N" dataDxfId="13"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="12"/>
+    <tableColumn id="1" name="#" dataDxfId="17"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="16"/>
+    <tableColumn id="5" name="G" dataDxfId="15"/>
+    <tableColumn id="3" name="N" dataDxfId="14"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A124:E134" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A124:E134"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A125:E135" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="A125:E135"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="10"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="9"/>
-    <tableColumn id="5" name="G" dataDxfId="8"/>
-    <tableColumn id="3" name="N" dataDxfId="7"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="6"/>
+    <tableColumn id="1" name="#" dataDxfId="11"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="10"/>
+    <tableColumn id="5" name="G" dataDxfId="9"/>
+    <tableColumn id="3" name="N" dataDxfId="8"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A36:E47" totalsRowShown="0" headerRowDxfId="105" headerRowBorderDxfId="104" tableBorderDxfId="103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A36:E47" totalsRowShown="0" headerRowDxfId="107" headerRowBorderDxfId="106" tableBorderDxfId="105">
   <autoFilter ref="A36:E47"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="102"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="101"/>
-    <tableColumn id="5" name="G" dataDxfId="100"/>
-    <tableColumn id="3" name="N" dataDxfId="99"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="98"/>
+    <tableColumn id="1" name="#" dataDxfId="104"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="103"/>
+    <tableColumn id="5" name="G" dataDxfId="102"/>
+    <tableColumn id="3" name="N" dataDxfId="101"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A95:E103" totalsRowShown="0" headerRowDxfId="97" headerRowBorderDxfId="96" tableBorderDxfId="95">
-  <autoFilter ref="A95:E103"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A96:E104" totalsRowShown="0" headerRowDxfId="99" headerRowBorderDxfId="98" tableBorderDxfId="97">
+  <autoFilter ref="A96:E104"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="94"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="93"/>
-    <tableColumn id="5" name="G" dataDxfId="92"/>
-    <tableColumn id="3" name="N" dataDxfId="91"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="90"/>
+    <tableColumn id="1" name="#" dataDxfId="96"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="95"/>
+    <tableColumn id="5" name="G" dataDxfId="94"/>
+    <tableColumn id="3" name="N" dataDxfId="93"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A106:E110" totalsRowShown="0" headerRowDxfId="89" headerRowBorderDxfId="88" tableBorderDxfId="87">
-  <autoFilter ref="A106:E110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A107:E111" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89">
+  <autoFilter ref="A107:E111"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="86"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="85"/>
-    <tableColumn id="5" name="G" dataDxfId="84"/>
-    <tableColumn id="3" name="N" dataDxfId="83"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="82"/>
+    <tableColumn id="1" name="#" dataDxfId="88"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="87"/>
+    <tableColumn id="5" name="G" dataDxfId="86"/>
+    <tableColumn id="3" name="N" dataDxfId="85"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A113:E121" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79">
-  <autoFilter ref="A113:E121"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A114:E122" totalsRowShown="0" headerRowDxfId="83" headerRowBorderDxfId="82" tableBorderDxfId="81">
+  <autoFilter ref="A114:E122"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="78"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="77"/>
-    <tableColumn id="5" name="G" dataDxfId="76"/>
-    <tableColumn id="3" name="N" dataDxfId="75"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="74"/>
+    <tableColumn id="1" name="#" dataDxfId="80"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="79"/>
+    <tableColumn id="5" name="G" dataDxfId="78"/>
+    <tableColumn id="3" name="N" dataDxfId="77"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A149:E163" totalsRowShown="0" headerRowDxfId="73">
-  <autoFilter ref="A149:E163"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A150:E164" totalsRowShown="0" headerRowDxfId="75">
+  <autoFilter ref="A150:E164"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="72"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="71"/>
-    <tableColumn id="5" name="G" dataDxfId="70"/>
-    <tableColumn id="3" name="N" dataDxfId="69"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="68"/>
+    <tableColumn id="1" name="#" dataDxfId="74"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="73"/>
+    <tableColumn id="5" name="G" dataDxfId="72"/>
+    <tableColumn id="3" name="N" dataDxfId="71"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A68:E73" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
-  <autoFilter ref="A68:E73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A69:E74" totalsRowShown="0" headerRowDxfId="69" headerRowBorderDxfId="68" tableBorderDxfId="67">
+  <autoFilter ref="A69:E74"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="64"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="63"/>
-    <tableColumn id="5" name="G" dataDxfId="62"/>
-    <tableColumn id="3" name="N" dataDxfId="61"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="60"/>
+    <tableColumn id="1" name="#" dataDxfId="66"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="65"/>
+    <tableColumn id="5" name="G" dataDxfId="64"/>
+    <tableColumn id="3" name="N" dataDxfId="63"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A50:E56" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58" tableBorderDxfId="57">
-  <autoFilter ref="A50:E56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A50:E57" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59">
+  <autoFilter ref="A50:E57"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="56"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="55"/>
-    <tableColumn id="5" name="G" dataDxfId="54"/>
-    <tableColumn id="3" name="N" dataDxfId="53"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="52"/>
+    <tableColumn id="1" name="#" dataDxfId="58"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="57"/>
+    <tableColumn id="5" name="G" dataDxfId="56"/>
+    <tableColumn id="3" name="N" dataDxfId="55"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="A166:E170" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
-  <autoFilter ref="A166:E170"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="A167:E171" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="52" tableBorderDxfId="51">
+  <autoFilter ref="A167:E171"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="48"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="47"/>
-    <tableColumn id="5" name="G" dataDxfId="46"/>
-    <tableColumn id="3" name="N" dataDxfId="45"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="44"/>
+    <tableColumn id="1" name="#" dataDxfId="50"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="49"/>
+    <tableColumn id="5" name="G" dataDxfId="48"/>
+    <tableColumn id="3" name="N" dataDxfId="47"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3739,10 +3846,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:F202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3751,7 +3858,7 @@
     <col min="2" max="2" width="120.85546875" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="56.28515625" style="61" customWidth="1"/>
+    <col min="5" max="5" width="57.42578125" style="61" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="73" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3801,7 +3908,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -3823,7 +3930,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C6" s="40">
         <v>5</v>
@@ -3844,7 +3951,7 @@
       </c>
       <c r="D7" s="41"/>
       <c r="E7" s="53" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F7" s="74"/>
     </row>
@@ -3869,7 +3976,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C9" s="40">
         <v>5</v>
@@ -3885,7 +3992,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C10" s="40">
         <v>5</v>
@@ -3931,7 +4038,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C13" s="40">
         <v>5</v>
@@ -4066,7 +4173,7 @@
       </c>
       <c r="D22" s="33"/>
       <c r="E22" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F22" s="74"/>
     </row>
@@ -4075,7 +4182,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C23" s="40">
         <v>5</v>
@@ -4117,7 +4224,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26" s="40">
         <v>5</v>
@@ -4131,7 +4238,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C27" s="40">
         <v>5</v>
@@ -4152,7 +4259,7 @@
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="43" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F28" s="74"/>
     </row>
@@ -4182,7 +4289,7 @@
       </c>
       <c r="D30" s="33"/>
       <c r="E30" s="43" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F30" s="74"/>
     </row>
@@ -4219,7 +4326,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="59" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C33" s="40">
         <v>5</v>
@@ -4281,7 +4388,7 @@
       </c>
       <c r="D37" s="33"/>
       <c r="E37" s="46" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F37" s="73"/>
     </row>
@@ -4406,7 +4513,7 @@
       <c r="D46" s="33"/>
       <c r="E46" s="43"/>
     </row>
-    <row r="47" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="26">
         <v>13</v>
       </c>
@@ -4418,7 +4525,7 @@
       </c>
       <c r="D47" s="33"/>
       <c r="E47" s="43" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="F47" s="73"/>
     </row>
@@ -4540,214 +4647,212 @@
       <c r="D56" s="33"/>
       <c r="E56" s="43"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="66"/>
-    </row>
-    <row r="58" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A58" s="23" t="s">
+    <row r="57" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="34"/>
+      <c r="D57" s="89"/>
+      <c r="E57" s="38"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="66"/>
+    </row>
+    <row r="59" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A59" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B59" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="28" t="s">
+      <c r="C59" s="8"/>
+      <c r="D59" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E58" s="63">
+      <c r="E59" s="63">
         <f>SUMPRODUCT(Table3[G],Table3[N])/SUM(Table3[G])</f>
         <v>0</v>
       </c>
-      <c r="F58" s="26"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+      <c r="F59" s="26"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B60" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C60" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D59" s="37" t="s">
+      <c r="D60" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="E59" s="35" t="s">
+      <c r="E60" s="35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
         <v>1</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C60" s="38">
+      <c r="C61" s="38">
         <v>9</v>
       </c>
-      <c r="D60" s="33"/>
-      <c r="E60" s="38" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="9">
-        <v>2</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C61" s="38">
-        <v>5</v>
-      </c>
       <c r="D61" s="33"/>
-      <c r="E61" s="38"/>
+      <c r="E61" s="38" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
+        <v>2</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C62" s="38">
+        <v>5</v>
+      </c>
+      <c r="D62" s="33"/>
+      <c r="E62" s="38"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="9">
         <v>3</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C62" s="38">
-        <v>5</v>
-      </c>
-      <c r="D62" s="33"/>
-      <c r="E62" s="38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
-        <v>4</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C63" s="38">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D63" s="33"/>
-      <c r="E63" s="38"/>
+      <c r="E63" s="38" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="38">
+        <v>9</v>
+      </c>
+      <c r="D64" s="33"/>
+      <c r="E64" s="38"/>
+    </row>
+    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>5</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C64" s="38">
-        <v>5</v>
-      </c>
-      <c r="D64" s="33"/>
-      <c r="E64" s="38" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
+      <c r="C65" s="38">
+        <v>5</v>
+      </c>
+      <c r="D65" s="33"/>
+      <c r="E65" s="38" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
         <v>6</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B66" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C65" s="38">
+      <c r="C66" s="38">
         <v>0</v>
       </c>
-      <c r="D65" s="33"/>
-      <c r="E65" s="38"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="66"/>
-    </row>
-    <row r="67" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A67" s="23" t="s">
+      <c r="D66" s="33"/>
+      <c r="E66" s="38" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="66"/>
+    </row>
+    <row r="68" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A68" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B68" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D67" s="28" t="s">
+      <c r="D68" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E67" s="63">
+      <c r="E68" s="63">
         <f>SUMPRODUCT(Table11[G],Table11[N])/SUM(Table11[G])</f>
         <v>0</v>
       </c>
-      <c r="F67" s="26"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+      <c r="F68" s="26"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B69" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="35" t="s">
+      <c r="C69" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D68" s="36" t="s">
+      <c r="D69" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E68" s="35" t="s">
+      <c r="E69" s="35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
-        <v>1</v>
-      </c>
-      <c r="B69" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69" s="34">
-        <v>5</v>
-      </c>
-      <c r="D69" s="33"/>
-      <c r="E69" s="38"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
+        <v>1</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="34">
+        <v>5</v>
+      </c>
+      <c r="D70" s="33"/>
+      <c r="E70" s="38"/>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
         <v>2</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C70" s="34">
-        <v>5</v>
-      </c>
-      <c r="D70" s="33"/>
-      <c r="E70" s="38" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="9">
-        <v>3</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="C71" s="34">
         <v>5</v>
       </c>
       <c r="D71" s="33"/>
-      <c r="E71" s="38"/>
+      <c r="E71" s="38" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C72" s="34">
         <v>5</v>
@@ -4756,11 +4861,11 @@
       <c r="E72" s="38"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="5">
-        <v>5</v>
+      <c r="A73" s="9">
+        <v>4</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="C73" s="34">
         <v>5</v>
@@ -4768,68 +4873,71 @@
       <c r="D73" s="33"/>
       <c r="E73" s="38"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="66"/>
+    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
+        <v>5</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C74" s="34">
+        <v>5</v>
+      </c>
+      <c r="D74" s="33"/>
+      <c r="E74" s="38"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="66"/>
     </row>
-    <row r="76" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A76" s="23" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="66"/>
+    </row>
+    <row r="77" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A77" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B77" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D76" s="28" t="s">
+      <c r="D77" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E76" s="63">
+      <c r="E77" s="63">
         <f>SUMPRODUCT(Table71518[G],Table71518[N])/SUM(Table71518[G])</f>
         <v>0</v>
       </c>
-      <c r="F76" s="26"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+      <c r="F77" s="26"/>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B78" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C77" s="35" t="s">
+      <c r="C78" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D77" s="36" t="s">
+      <c r="D78" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E77" s="35" t="s">
+      <c r="E78" s="35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="5">
-        <v>1</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C78" s="34">
-        <v>5</v>
-      </c>
-      <c r="D78" s="33"/>
-      <c r="E78" s="38"/>
+      <c r="F78" s="88" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C79" s="34">
         <v>5</v>
@@ -4838,103 +4946,120 @@
       <c r="E79" s="38"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="9">
-        <v>3</v>
+      <c r="A80" s="5">
+        <v>2</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="C80" s="34">
         <v>5</v>
       </c>
       <c r="D80" s="33"/>
       <c r="E80" s="38"/>
-    </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F80" s="73" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="C81" s="34">
         <v>5</v>
       </c>
       <c r="D81" s="33"/>
       <c r="E81" s="38"/>
-    </row>
-    <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="5">
-        <v>5</v>
+      <c r="F81" s="73" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="9">
+        <v>4</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C82" s="34">
+        <v>5</v>
+      </c>
+      <c r="D82" s="33"/>
+      <c r="E82" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="F82" s="73" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="5">
+        <v>5</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C82" s="34">
-        <v>5</v>
-      </c>
-      <c r="D82" s="33"/>
-      <c r="E82" s="38"/>
-    </row>
-    <row r="84" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B84"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
-      <c r="E84" s="68"/>
-      <c r="F84" s="26"/>
-    </row>
-    <row r="85" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A85" s="23" t="s">
+      <c r="C83" s="34">
+        <v>5</v>
+      </c>
+      <c r="D83" s="33"/>
+      <c r="E83" s="38"/>
+      <c r="F83" s="73" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B85"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="68"/>
+      <c r="F85" s="26"/>
+    </row>
+    <row r="86" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A86" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B85" s="10" t="s">
+      <c r="B86" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C85" s="1"/>
-      <c r="D85" s="28" t="s">
+      <c r="C86" s="1"/>
+      <c r="D86" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E85" s="63">
+      <c r="E86" s="63">
         <f>SUMPRODUCT(Table715[G],Table715[N])/SUM(Table715[G])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+    <row r="87" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B87" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C86" s="35" t="s">
+      <c r="C87" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D86" s="36" t="s">
+      <c r="D87" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E86" s="35" t="s">
+      <c r="E87" s="35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="5">
-        <v>1</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C87" s="38">
-        <v>5</v>
-      </c>
-      <c r="D87" s="33"/>
-      <c r="E87" s="38"/>
+      <c r="F87" s="87" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="C88" s="38">
         <v>5</v>
@@ -4943,24 +5068,25 @@
       <c r="E88" s="38"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="9">
-        <v>3</v>
+      <c r="A89" s="5">
+        <v>2</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>170</v>
+        <v>117</v>
       </c>
       <c r="C89" s="38">
         <v>5</v>
       </c>
       <c r="D89" s="33"/>
       <c r="E89" s="38"/>
+      <c r="F89" s="86"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>35</v>
+        <v>167</v>
       </c>
       <c r="C90" s="38">
         <v>5</v>
@@ -4969,11 +5095,11 @@
       <c r="E90" s="38"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="5">
-        <v>5</v>
+      <c r="A91" s="9">
+        <v>4</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>169</v>
+        <v>35</v>
       </c>
       <c r="C91" s="38">
         <v>5</v>
@@ -4983,76 +5109,82 @@
     </row>
     <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>50</v>
+        <v>166</v>
       </c>
       <c r="C92" s="38">
         <v>5</v>
       </c>
       <c r="D92" s="33"/>
       <c r="E92" s="38"/>
-    </row>
-    <row r="93" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B93"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="68"/>
-      <c r="F93" s="26"/>
-    </row>
-    <row r="94" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A94" s="23" t="s">
+      <c r="F92" s="86">
+        <v>40826</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <v>6</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C93" s="38">
+        <v>5</v>
+      </c>
+      <c r="D93" s="33"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="86">
+        <v>40826</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B94"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="68"/>
+      <c r="F94" s="26"/>
+    </row>
+    <row r="95" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A95" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B94" s="10" t="s">
+      <c r="B95" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C94" s="1"/>
-      <c r="D94" s="28" t="s">
+      <c r="C95" s="1"/>
+      <c r="D95" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E94" s="63">
+      <c r="E95" s="63">
         <f>SUMPRODUCT(Table7[G],Table7[N])/SUM(Table7[G])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B96" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C95" s="35" t="s">
+      <c r="C96" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D95" s="36" t="s">
+      <c r="D96" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E95" s="35" t="s">
+      <c r="E96" s="35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="5">
-        <v>1</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C96" s="34">
-        <v>5</v>
-      </c>
-      <c r="D96" s="33"/>
-      <c r="E96" s="38"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
-        <v>2</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>132</v>
+        <v>1</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C97" s="34">
         <v>5</v>
@@ -5060,25 +5192,27 @@
       <c r="D97" s="33"/>
       <c r="E97" s="38"/>
     </row>
-    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
-        <v>3</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>114</v>
+        <v>2</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="C98" s="34">
         <v>5</v>
       </c>
       <c r="D98" s="33"/>
-      <c r="E98" s="38"/>
+      <c r="E98" s="38" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C99" s="34">
         <v>5</v>
@@ -5087,24 +5221,24 @@
       <c r="E99" s="38"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="9">
-        <v>5</v>
+      <c r="A100" s="5">
+        <v>4</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>171</v>
+        <v>131</v>
       </c>
       <c r="C100" s="34">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D100" s="33"/>
       <c r="E100" s="38"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>36</v>
+        <v>168</v>
       </c>
       <c r="C101" s="34">
         <v>0</v>
@@ -5114,117 +5248,117 @@
     </row>
     <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
+        <v>6</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C102" s="34">
+        <v>0</v>
+      </c>
+      <c r="D102" s="33"/>
+      <c r="E102" s="38"/>
+    </row>
+    <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="9">
         <v>7</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="34">
-        <v>5</v>
-      </c>
-      <c r="D102" s="33"/>
-      <c r="E102" s="38" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="5">
+      <c r="B103" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="34">
+        <v>5</v>
+      </c>
+      <c r="D103" s="33"/>
+      <c r="E103" s="38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="5">
         <v>8</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C103" s="34">
-        <v>5</v>
-      </c>
-      <c r="D103" s="33"/>
-      <c r="E103" s="38"/>
-    </row>
-    <row r="104" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B104" s="56"/>
-      <c r="C104" s="34"/>
-      <c r="D104" s="57"/>
-      <c r="E104" s="69"/>
-      <c r="F104" s="26"/>
-    </row>
-    <row r="105" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A105" s="23" t="s">
+      <c r="C104" s="34">
+        <v>5</v>
+      </c>
+      <c r="D104" s="33"/>
+      <c r="E104" s="38"/>
+    </row>
+    <row r="105" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B105" s="56"/>
+      <c r="C105" s="34"/>
+      <c r="D105" s="57"/>
+      <c r="E105" s="69"/>
+      <c r="F105" s="26"/>
+    </row>
+    <row r="106" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A106" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B105" s="10" t="s">
+      <c r="B106" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C105" s="1"/>
-      <c r="D105" s="28" t="s">
+      <c r="C106" s="1"/>
+      <c r="D106" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="63">
+      <c r="E106" s="63">
         <f>SUMPRODUCT(Table8[G],Table8[N])/SUM(Table8[G])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B107" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C106" s="35" t="s">
+      <c r="C107" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D106" s="36" t="s">
+      <c r="D107" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E106" s="35" t="s">
+      <c r="E107" s="35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="5">
-        <v>1</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C107" s="34">
-        <v>5</v>
-      </c>
-      <c r="D107" s="33"/>
-      <c r="E107" s="38"/>
     </row>
     <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C108" s="34">
         <v>5</v>
       </c>
       <c r="D108" s="33"/>
-      <c r="E108" s="67"/>
+      <c r="E108" s="38"/>
     </row>
     <row r="109" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="C109" s="34">
         <v>5</v>
       </c>
       <c r="D109" s="33"/>
-      <c r="E109" s="38"/>
+      <c r="E109" s="67"/>
     </row>
     <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
       <c r="C110" s="34">
         <v>5</v>
@@ -5232,65 +5366,65 @@
       <c r="D110" s="33"/>
       <c r="E110" s="38"/>
     </row>
-    <row r="111" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B111" s="56"/>
-      <c r="C111" s="34"/>
-      <c r="D111" s="57"/>
-      <c r="E111" s="69"/>
-      <c r="F111" s="26"/>
-    </row>
-    <row r="112" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A112" s="23" t="s">
+    <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="5">
+        <v>4</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C111" s="34">
+        <v>5</v>
+      </c>
+      <c r="D111" s="33"/>
+      <c r="E111" s="38"/>
+    </row>
+    <row r="112" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B112" s="56"/>
+      <c r="C112" s="34"/>
+      <c r="D112" s="57"/>
+      <c r="E112" s="69"/>
+      <c r="F112" s="26"/>
+    </row>
+    <row r="113" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A113" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B112" s="10" t="s">
+      <c r="B113" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C112" s="1"/>
-      <c r="D112" s="28" t="s">
+      <c r="C113" s="1"/>
+      <c r="D113" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E112" s="63">
+      <c r="E113" s="63">
         <f>SUMPRODUCT(Table9[G],Table9[N])/SUM(Table9[G])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="B114" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C113" s="35" t="s">
+      <c r="C114" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D113" s="36" t="s">
+      <c r="D114" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E113" s="35" t="s">
+      <c r="E114" s="35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="5">
-        <v>1</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C114" s="34">
-        <v>5</v>
-      </c>
-      <c r="D114" s="33"/>
-      <c r="E114" s="38"/>
     </row>
     <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="C115" s="34">
         <v>5</v>
@@ -5300,10 +5434,10 @@
     </row>
     <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="C116" s="34">
         <v>5</v>
@@ -5311,25 +5445,27 @@
       <c r="D116" s="33"/>
       <c r="E116" s="38"/>
     </row>
-    <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="9">
-        <v>4</v>
+    <row r="117" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="5">
+        <v>3</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C117" s="34">
         <v>5</v>
       </c>
       <c r="D117" s="33"/>
-      <c r="E117" s="38"/>
+      <c r="E117" s="38" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C118" s="34">
         <v>5</v>
@@ -5339,10 +5475,10 @@
     </row>
     <row r="119" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="9">
+        <v>5</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C119" s="34">
         <v>5</v>
@@ -5351,11 +5487,11 @@
       <c r="E119" s="38"/>
     </row>
     <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="5">
-        <v>7</v>
+      <c r="A120" s="9">
+        <v>6</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>7</v>
+        <v>119</v>
       </c>
       <c r="C120" s="34">
         <v>5</v>
@@ -5365,76 +5501,80 @@
     </row>
     <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
+        <v>7</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" s="34">
+        <v>5</v>
+      </c>
+      <c r="D121" s="33"/>
+      <c r="E121" s="38" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="5">
         <v>8</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C121" s="34">
-        <v>5</v>
-      </c>
-      <c r="D121" s="33"/>
-      <c r="E121" s="38"/>
-    </row>
-    <row r="122" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B122"/>
-      <c r="C122" s="7"/>
-      <c r="D122" s="7"/>
-      <c r="E122" s="68"/>
-      <c r="F122" s="26"/>
-    </row>
-    <row r="123" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A123" s="23" t="s">
+      <c r="C122" s="34">
+        <v>5</v>
+      </c>
+      <c r="D122" s="33"/>
+      <c r="E122" s="38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B123"/>
+      <c r="C123" s="7"/>
+      <c r="D123" s="7"/>
+      <c r="E123" s="68"/>
+      <c r="F123" s="26"/>
+    </row>
+    <row r="124" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A124" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B123" s="10" t="s">
+      <c r="B124" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C123" s="1"/>
-      <c r="D123" s="28" t="s">
+      <c r="C124" s="1"/>
+      <c r="D124" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E123" s="63">
+      <c r="E124" s="63">
         <f>SUMPRODUCT(Table1021[G],Table1021[N])/SUM(Table1021[G])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B125" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C124" s="35" t="s">
+      <c r="C125" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D124" s="36" t="s">
+      <c r="D125" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E124" s="35" t="s">
+      <c r="E125" s="35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A125" s="5">
-        <v>1</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C125" s="34">
-        <v>5</v>
-      </c>
-      <c r="D125" s="33"/>
-      <c r="E125" s="38"/>
     </row>
     <row r="126" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
-        <v>2</v>
-      </c>
-      <c r="B126" s="16" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C126" s="34">
         <v>5</v>
@@ -5442,81 +5582,81 @@
       <c r="D126" s="33"/>
       <c r="E126" s="38"/>
     </row>
-    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A127" s="9">
+    <row r="127" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A127" s="5">
+        <v>2</v>
+      </c>
+      <c r="B127" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C127" s="34">
+        <v>5</v>
+      </c>
+      <c r="D127" s="33"/>
+      <c r="E127" s="38"/>
+    </row>
+    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="9">
         <v>3</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C127" s="34"/>
-      <c r="D127" s="33"/>
-      <c r="E127" s="38" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A128" s="9">
-        <v>4</v>
-      </c>
-      <c r="B128" s="56" t="s">
-        <v>134</v>
-      </c>
-      <c r="C128" s="34">
-        <v>5</v>
-      </c>
+      <c r="C128" s="34"/>
       <c r="D128" s="33"/>
-      <c r="E128" s="38"/>
+      <c r="E128" s="38" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="129" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="9">
-        <v>5</v>
-      </c>
-      <c r="B129" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B129" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="C129" s="34">
+        <v>5</v>
+      </c>
+      <c r="D129" s="33"/>
+      <c r="E129" s="38"/>
+    </row>
+    <row r="130" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A130" s="9">
+        <v>5</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C129" s="34">
-        <v>5</v>
-      </c>
-      <c r="D129" s="33"/>
-      <c r="E129" s="38" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A130" s="5">
-        <v>6</v>
-      </c>
-      <c r="B130" s="16" t="s">
-        <v>49</v>
       </c>
       <c r="C130" s="34">
         <v>5</v>
       </c>
       <c r="D130" s="33"/>
       <c r="E130" s="38" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
+        <v>6</v>
+      </c>
+      <c r="B131" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C131" s="34">
+        <v>5</v>
+      </c>
+      <c r="D131" s="33"/>
+      <c r="E131" s="38" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="5">
         <v>7</v>
       </c>
-      <c r="B131" s="16" t="s">
+      <c r="B132" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="C131" s="34">
-        <v>5</v>
-      </c>
-      <c r="D131" s="33"/>
-      <c r="E131" s="38"/>
-    </row>
-    <row r="132" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A132" s="5">
-        <v>8</v>
-      </c>
-      <c r="B132" s="56" t="s">
-        <v>135</v>
       </c>
       <c r="C132" s="34">
         <v>5</v>
@@ -5525,11 +5665,11 @@
       <c r="E132" s="38"/>
     </row>
     <row r="133" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="9">
-        <v>9</v>
-      </c>
-      <c r="B133" s="16" t="s">
-        <v>23</v>
+      <c r="A133" s="5">
+        <v>8</v>
+      </c>
+      <c r="B133" s="56" t="s">
+        <v>135</v>
       </c>
       <c r="C133" s="34">
         <v>5</v>
@@ -5537,93 +5677,95 @@
       <c r="D133" s="33"/>
       <c r="E133" s="38"/>
     </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134" s="26">
+    <row r="134" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A134" s="9">
+        <v>9</v>
+      </c>
+      <c r="B134" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C134" s="34">
+        <v>5</v>
+      </c>
+      <c r="D134" s="33"/>
+      <c r="E134" s="38"/>
+    </row>
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="26">
         <v>10</v>
       </c>
-      <c r="B134" s="16" t="s">
+      <c r="B135" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C134" s="34">
-        <v>5</v>
-      </c>
-      <c r="D134" s="33"/>
-      <c r="E134" s="38" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B135"/>
-      <c r="C135" s="7"/>
-      <c r="D135" s="7"/>
-      <c r="E135" s="68"/>
-      <c r="F135" s="26"/>
-    </row>
-    <row r="136" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A136" s="23" t="s">
+      <c r="C135" s="34">
+        <v>5</v>
+      </c>
+      <c r="D135" s="33"/>
+      <c r="E135" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B136"/>
+      <c r="C136" s="7"/>
+      <c r="D136" s="7"/>
+      <c r="E136" s="68"/>
+      <c r="F136" s="26"/>
+    </row>
+    <row r="137" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A137" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B136" s="10" t="s">
+      <c r="B137" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C136" s="1"/>
-      <c r="D136" s="28" t="s">
+      <c r="C137" s="1"/>
+      <c r="D137" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E136" s="63">
+      <c r="E137" s="63">
         <f>SUMPRODUCT(Table1020[G],Table1020[N])/SUM(Table1020[G])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="5" t="s">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B137" s="5" t="s">
+      <c r="B138" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C137" s="35" t="s">
+      <c r="C138" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D137" s="36" t="s">
+      <c r="D138" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E137" s="35" t="s">
+      <c r="E138" s="35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A138" s="5">
+    <row r="139" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A139" s="5">
         <v>1</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B139" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C138" s="34">
-        <v>5</v>
-      </c>
-      <c r="D138" s="33"/>
-      <c r="E138" s="38"/>
-    </row>
-    <row r="139" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" s="9">
-        <v>2</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C139" s="34">
         <v>5</v>
       </c>
       <c r="D139" s="33"/>
-      <c r="E139" s="38"/>
+      <c r="E139" s="38" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="140" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="9">
-        <v>3</v>
-      </c>
-      <c r="B140" s="16" t="s">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C140" s="34">
         <v>5</v>
@@ -5633,10 +5775,10 @@
     </row>
     <row r="141" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C141" s="34">
         <v>5</v>
@@ -5645,52 +5787,52 @@
       <c r="E141" s="38"/>
     </row>
     <row r="142" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A142" s="76">
-        <v>5</v>
-      </c>
-      <c r="B142" s="77" t="s">
+      <c r="A142" s="9">
+        <v>4</v>
+      </c>
+      <c r="B142" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C142" s="34">
+        <v>5</v>
+      </c>
+      <c r="D142" s="33"/>
+      <c r="E142" s="38"/>
+    </row>
+    <row r="143" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A143" s="76">
+        <v>5</v>
+      </c>
+      <c r="B143" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="C142" s="78">
+      <c r="C143" s="78">
         <v>0</v>
       </c>
-      <c r="D142" s="79"/>
-      <c r="E142" s="80" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A143" s="5">
-        <v>6</v>
-      </c>
-      <c r="B143" t="s">
-        <v>136</v>
-      </c>
-      <c r="C143" s="34"/>
-      <c r="D143" s="33"/>
-      <c r="E143" s="38" t="s">
-        <v>173</v>
+      <c r="D143" s="79"/>
+      <c r="E143" s="80" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
+        <v>6</v>
+      </c>
+      <c r="B144" t="s">
+        <v>136</v>
+      </c>
+      <c r="C144" s="34"/>
+      <c r="D144" s="33"/>
+      <c r="E144" s="38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A145" s="5">
         <v>7</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B145" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C144" s="34">
-        <v>5</v>
-      </c>
-      <c r="D144" s="33"/>
-      <c r="E144" s="38"/>
-    </row>
-    <row r="145" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A145" s="9">
-        <v>8</v>
-      </c>
-      <c r="B145" s="16" t="s">
-        <v>13</v>
       </c>
       <c r="C145" s="34">
         <v>5</v>
@@ -5698,98 +5840,100 @@
       <c r="D145" s="33"/>
       <c r="E145" s="38"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C146" s="7"/>
-      <c r="D146" s="7"/>
-      <c r="E146" s="66"/>
-    </row>
-    <row r="147" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B147"/>
+    <row r="146" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A146" s="9">
+        <v>8</v>
+      </c>
+      <c r="B146" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C146" s="34">
+        <v>5</v>
+      </c>
+      <c r="D146" s="33"/>
+      <c r="E146" s="38"/>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
-      <c r="E147" s="68"/>
-      <c r="F147" s="26"/>
-    </row>
-    <row r="148" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A148" s="23" t="s">
+      <c r="E147" s="66"/>
+    </row>
+    <row r="148" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B148"/>
+      <c r="C148" s="7"/>
+      <c r="D148" s="7"/>
+      <c r="E148" s="68"/>
+      <c r="F148" s="26"/>
+    </row>
+    <row r="149" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A149" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="B148" s="10" t="s">
+      <c r="B149" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C148" s="1"/>
-      <c r="D148" s="28" t="s">
+      <c r="C149" s="1"/>
+      <c r="D149" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E148" s="63">
+      <c r="E149" s="63">
         <f>SUMPRODUCT(Table10[G],Table10[N])/SUM(Table10[G])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B149" s="5" t="s">
+      <c r="B150" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C149" s="35" t="s">
+      <c r="C150" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D149" s="36" t="s">
+      <c r="D150" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E149" s="35" t="s">
+      <c r="E150" s="35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="20">
+    <row r="151" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A151" s="20">
         <v>1</v>
       </c>
-      <c r="B150" s="16" t="s">
+      <c r="B151" s="16" t="s">
         <v>25</v>
-      </c>
-      <c r="C150" s="34">
-        <v>5</v>
-      </c>
-      <c r="D150" s="33"/>
-      <c r="E150" s="38"/>
-    </row>
-    <row r="151" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="5">
-        <v>2</v>
-      </c>
-      <c r="B151" t="s">
-        <v>19</v>
       </c>
       <c r="C151" s="34">
         <v>5</v>
       </c>
       <c r="D151" s="33"/>
       <c r="E151" s="38" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
+        <v>2</v>
+      </c>
+      <c r="B152" t="s">
+        <v>19</v>
+      </c>
+      <c r="C152" s="34">
+        <v>5</v>
+      </c>
+      <c r="D152" s="33"/>
+      <c r="E152" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A153" s="5">
         <v>3</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B153" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C152" s="34">
-        <v>5</v>
-      </c>
-      <c r="D152" s="33"/>
-      <c r="E152" s="38"/>
-    </row>
-    <row r="153" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="9">
-        <v>4</v>
-      </c>
-      <c r="B153" s="16" t="s">
-        <v>46</v>
       </c>
       <c r="C153" s="34">
         <v>5</v>
@@ -5799,10 +5943,10 @@
     </row>
     <row r="154" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="9">
-        <v>5</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
+      </c>
+      <c r="B154" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="C154" s="34">
         <v>5</v>
@@ -5810,81 +5954,83 @@
       <c r="D154" s="33"/>
       <c r="E154" s="38"/>
     </row>
-    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A155" s="5">
+    <row r="155" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A155" s="9">
+        <v>5</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C155" s="34">
+        <v>5</v>
+      </c>
+      <c r="D155" s="33"/>
+      <c r="E155" s="38"/>
+    </row>
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" s="5">
         <v>6</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B156" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C155" s="34">
-        <v>5</v>
-      </c>
-      <c r="D155" s="33"/>
-      <c r="E155" s="52"/>
-    </row>
-    <row r="156" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="9">
+      <c r="C156" s="34">
+        <v>5</v>
+      </c>
+      <c r="D156" s="33"/>
+      <c r="E156" s="52" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A157" s="9">
         <v>7</v>
       </c>
-      <c r="B156" s="16" t="s">
+      <c r="B157" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="C156" s="34">
-        <v>5</v>
-      </c>
-      <c r="D156" s="33"/>
-      <c r="E156" s="38" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A157" s="9">
-        <v>8</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="C157" s="34">
         <v>5</v>
       </c>
       <c r="D157" s="33"/>
       <c r="E157" s="38" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="9">
-        <v>9</v>
-      </c>
-      <c r="B158" s="16" t="s">
-        <v>44</v>
+        <v>8</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C158" s="34">
         <v>5</v>
       </c>
       <c r="D158" s="33"/>
-      <c r="E158" s="52"/>
+      <c r="E158" s="38" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="159" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="9">
+        <v>9</v>
+      </c>
+      <c r="B159" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C159" s="34">
+        <v>5</v>
+      </c>
+      <c r="D159" s="33"/>
+      <c r="E159" s="52"/>
+    </row>
+    <row r="160" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A160" s="9">
         <v>10</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B160" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C159" s="34">
-        <v>5</v>
-      </c>
-      <c r="D159" s="33"/>
-      <c r="E159" s="38"/>
-    </row>
-    <row r="160" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="20">
-        <v>11</v>
-      </c>
-      <c r="B160" s="16" t="s">
-        <v>45</v>
       </c>
       <c r="C160" s="34">
         <v>5</v>
@@ -5893,11 +6039,11 @@
       <c r="E160" s="38"/>
     </row>
     <row r="161" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="60">
-        <v>12</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>124</v>
+      <c r="A161" s="20">
+        <v>11</v>
+      </c>
+      <c r="B161" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="C161" s="34">
         <v>5</v>
@@ -5906,11 +6052,11 @@
       <c r="E161" s="38"/>
     </row>
     <row r="162" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="26">
-        <v>13</v>
+      <c r="A162" s="60">
+        <v>12</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C162" s="34">
         <v>5</v>
@@ -5920,10 +6066,10 @@
     </row>
     <row r="163" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="26">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C163" s="34">
         <v>5</v>
@@ -5931,78 +6077,78 @@
       <c r="D163" s="33"/>
       <c r="E163" s="38"/>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C164" s="7"/>
-      <c r="D164" s="7"/>
-      <c r="E164" s="66"/>
-    </row>
-    <row r="165" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A165" s="23" t="s">
+    <row r="164" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A164" s="26">
+        <v>14</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C164" s="34">
+        <v>5</v>
+      </c>
+      <c r="D164" s="33"/>
+      <c r="E164" s="38"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C165" s="7"/>
+      <c r="D165" s="7"/>
+      <c r="E165" s="66"/>
+    </row>
+    <row r="166" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A166" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="B165" s="10" t="s">
+      <c r="B166" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C165" s="7"/>
-      <c r="D165" s="28" t="s">
+      <c r="C166" s="7"/>
+      <c r="D166" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E165" s="63">
+      <c r="E166" s="63">
         <f>SUMPRODUCT(Table15[G],Table15[N])/SUM(Table15[G])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B166" s="5" t="s">
+      <c r="B167" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C166" s="35" t="s">
+      <c r="C167" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D166" s="36" t="s">
+      <c r="D167" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E166" s="35" t="s">
+      <c r="E167" s="35" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A167" s="5">
-        <v>1</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C167" s="34">
-        <v>5</v>
-      </c>
-      <c r="D167" s="33"/>
-      <c r="E167" s="38" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>128</v>
+        <v>14</v>
       </c>
       <c r="C168" s="34">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D168" s="33"/>
-      <c r="E168" s="38"/>
+      <c r="E168" s="38" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="169" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C169" s="34">
         <v>0</v>
@@ -6011,11 +6157,11 @@
       <c r="E169" s="38"/>
     </row>
     <row r="170" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A170" s="9">
-        <v>4</v>
-      </c>
-      <c r="B170" s="56" t="s">
-        <v>129</v>
+      <c r="A170" s="5">
+        <v>3</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C170" s="34">
         <v>0</v>
@@ -6023,74 +6169,68 @@
       <c r="D170" s="33"/>
       <c r="E170" s="38"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C171" s="7"/>
-      <c r="D171" s="7"/>
-      <c r="E171" s="66"/>
-    </row>
-    <row r="173" spans="1:6" s="55" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A173" s="54" t="s">
+    <row r="171" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A171" s="9">
+        <v>4</v>
+      </c>
+      <c r="B171" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="C171" s="34">
+        <v>0</v>
+      </c>
+      <c r="D171" s="33"/>
+      <c r="E171" s="38"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C172" s="7"/>
+      <c r="D172" s="7"/>
+      <c r="E172" s="66"/>
+    </row>
+    <row r="174" spans="1:6" s="55" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A174" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="E173" s="70"/>
-      <c r="F173" s="81" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A174" s="24" t="s">
+      <c r="E174" s="70"/>
+      <c r="F174" s="81" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A175" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="B174" s="17" t="s">
+      <c r="B175" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C174" s="27"/>
-      <c r="D174" s="28" t="s">
+      <c r="C175" s="27"/>
+      <c r="D175" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E174" s="63">
+      <c r="E175" s="63">
         <f>SUMPRODUCT(Table2[G],Table2[N])/SUM(Table2[G])</f>
         <v>0</v>
       </c>
-      <c r="F174" s="81">
+      <c r="F175" s="81">
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F175" s="81"/>
-    </row>
     <row r="176" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A176" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="B176" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C176" s="10"/>
-      <c r="D176" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="E176" s="71">
-        <f>SUMPRODUCT(Table6[G],Table6[N])/SUM(Table6[G])</f>
-        <v>0</v>
-      </c>
-      <c r="F176" s="81">
-        <v>3</v>
-      </c>
+      <c r="F176" s="81"/>
     </row>
     <row r="177" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A177" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C177" s="10"/>
       <c r="D177" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E177" s="71">
-        <f>SUMPRODUCT(Table12[G],Table12[N])/SUM(Table12[G])</f>
+        <f>SUMPRODUCT(Table6[G],Table6[N])/SUM(Table6[G])</f>
         <v>0</v>
       </c>
       <c r="F177" s="81">
@@ -6099,92 +6239,92 @@
     </row>
     <row r="178" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A178" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B178" s="10" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C178" s="10"/>
       <c r="D178" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E178" s="71">
+        <f>SUMPRODUCT(Table12[G],Table12[N])/SUM(Table12[G])</f>
+        <v>0</v>
+      </c>
+      <c r="F178" s="81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A179" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B179" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C179" s="10"/>
+      <c r="D179" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E179" s="71">
         <f>SUMPRODUCT(Table3[G],Table3[N])/SUM(Table3[G])</f>
         <v>0</v>
       </c>
-      <c r="F178" s="81">
+      <c r="F179" s="81">
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A179" s="47">
+    <row r="180" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A180" s="47">
         <v>2</v>
       </c>
-      <c r="B179" s="48" t="s">
+      <c r="B180" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="E179" s="72">
-        <f>SUMPRODUCT(F176:F178,E176:E178)/SUM(F176:F178)</f>
+      <c r="E180" s="72">
+        <f>SUMPRODUCT(F177:F179,E177:E179)/SUM(F177:F179)</f>
         <v>0</v>
       </c>
-      <c r="F179" s="81">
+      <c r="F180" s="81">
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F180" s="81"/>
-    </row>
     <row r="181" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A181" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="B181" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C181" s="10"/>
-      <c r="D181" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="E181" s="71">
-        <f>SUMPRODUCT(Table11[G],Table11[N])/SUM(Table11[G])</f>
-        <v>0</v>
-      </c>
-      <c r="F181" s="81">
-        <v>4</v>
-      </c>
+      <c r="F181" s="81"/>
     </row>
     <row r="182" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B182" s="10" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C182" s="10"/>
       <c r="D182" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E182" s="71">
-        <f>SUMPRODUCT(Table71518[G],Table71518[N])/SUM(Table71518[G])</f>
+        <f>SUMPRODUCT(Table11[G],Table11[N])/SUM(Table11[G])</f>
         <v>0</v>
       </c>
       <c r="F182" s="81">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B183" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C183" s="10"/>
       <c r="D183" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E183" s="71">
-        <f>SUMPRODUCT(Table715[G],Table715[N])/SUM(Table715[G])</f>
+        <f>SUMPRODUCT(Table71518[G],Table71518[N])/SUM(Table71518[G])</f>
         <v>0</v>
       </c>
       <c r="F183" s="81">
@@ -6193,55 +6333,55 @@
     </row>
     <row r="184" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A184" s="49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B184" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C184" s="10"/>
       <c r="D184" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E184" s="71">
-        <f>SUMPRODUCT(Table7[G],Table7[N])/SUM(Table7[G])</f>
+        <f>SUMPRODUCT(Table715[G],Table715[N])/SUM(Table715[G])</f>
         <v>0</v>
       </c>
       <c r="F184" s="81">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A185" s="49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B185" s="10" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="C185" s="10"/>
       <c r="D185" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E185" s="71">
-        <f>SUMPRODUCT(Table8[G],Table8[N])/SUM(Table8[G])</f>
+        <f>SUMPRODUCT(Table7[G],Table7[N])/SUM(Table7[G])</f>
         <v>0</v>
       </c>
       <c r="F185" s="81">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A186" s="49" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C186" s="10"/>
       <c r="D186" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E186" s="71">
-        <f>SUMPRODUCT(Table9[G],Table9[N])/SUM(Table9[G])</f>
+        <f>SUMPRODUCT(Table8[G],Table8[N])/SUM(Table8[G])</f>
         <v>0</v>
       </c>
       <c r="F186" s="81">
@@ -6250,122 +6390,141 @@
     </row>
     <row r="187" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A187" s="49" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B187" s="10" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C187" s="10"/>
       <c r="D187" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E187" s="71">
-        <f>SUMPRODUCT(Table1021[G],Table1021[N])/SUM(Table1021[G])</f>
+        <f>SUMPRODUCT(Table9[G],Table9[N])/SUM(Table9[G])</f>
         <v>0</v>
       </c>
       <c r="F187" s="81">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A188" s="49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B188" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C188" s="10"/>
       <c r="D188" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E188" s="71">
-        <f>SUMPRODUCT(Table1020[G],Table1020[N])/SUM(Table1020[G])</f>
+        <f>SUMPRODUCT(Table1021[G],Table1021[N])/SUM(Table1021[G])</f>
         <v>0</v>
       </c>
       <c r="F188" s="81">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A189" s="49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C189" s="10"/>
       <c r="D189" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E189" s="71">
+        <f>SUMPRODUCT(Table1020[G],Table1020[N])/SUM(Table1020[G])</f>
+        <v>0</v>
+      </c>
+      <c r="F189" s="81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A190" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B190" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C190" s="10"/>
+      <c r="D190" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E190" s="71">
         <f>SUMPRODUCT(Table10[G],Table10[N])/SUM(Table10[G])</f>
         <v>0</v>
       </c>
-      <c r="F189" s="81">
+      <c r="F190" s="81">
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A190" s="49" t="s">
+    <row r="191" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A191" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="B190" s="10" t="s">
+      <c r="B191" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C190" s="51"/>
-      <c r="D190" s="50" t="s">
+      <c r="C191" s="51"/>
+      <c r="D191" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E190" s="71">
+      <c r="E191" s="71">
         <v>0</v>
       </c>
-      <c r="F190" s="81">
+      <c r="F191" s="81">
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A191" s="47">
+    <row r="192" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A192" s="47">
         <v>2</v>
       </c>
-      <c r="B191" s="48" t="s">
+      <c r="B192" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="E191" s="72">
-        <f>SUMPRODUCT(F181:F190,E181:E190)/SUM(F181:F190)</f>
+      <c r="E192" s="72">
+        <f>SUMPRODUCT(F182:F191,E182:E191)/SUM(F182:F191)</f>
         <v>0</v>
       </c>
-      <c r="F191" s="81">
+      <c r="F192" s="81">
         <v>3</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F192" s="81"/>
     </row>
     <row r="193" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F193" s="81"/>
     </row>
     <row r="194" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B194" t="s">
+      <c r="F194" s="81"/>
+    </row>
+    <row r="195" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B195" t="s">
         <v>102</v>
       </c>
-      <c r="E194" s="61">
-        <f>((E174*F174)+E179*F179+E191*F191)/(F174+F179+F191)</f>
+      <c r="E195" s="61">
+        <f>((E175*F175)+E180*F180+E192*F192)/(F175+F180+F192)</f>
         <v>0</v>
       </c>
-      <c r="F194" s="81"/>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="F195" s="81"/>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>